<commit_message>
final export json file feature
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quangtran/workspace/quangtran/source/website/qGetBagdeImage/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alphatheta/Documents/qExample/qGetBagdeImage/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D0A0C73-C9FB-9B48-816F-AE0AED5B1831}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B2ED84-6232-FA41-BFC5-44E6C0290995}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35380" windowHeight="17420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EmployeesList" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>No.</t>
   </si>
@@ -32,6 +32,12 @@
   </si>
   <si>
     <t>Position</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Project</t>
   </si>
 </sst>
 </file>
@@ -69,7 +75,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -92,18 +98,80 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -111,17 +179,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -461,161 +552,984 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:F95"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
     <col min="3" max="3" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="5" max="5" width="29.83203125" customWidth="1"/>
+    <col min="6" max="6" width="27.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="3"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="3"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="3"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="3"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="3"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="3"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="3"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="3"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="3"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="3"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="5"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="5"/>
+      <c r="E1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="5">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="5">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="11"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="5">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="11"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="5">
+        <v>13</v>
+      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="11"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="5">
+        <v>14</v>
+      </c>
+      <c r="B15" s="12"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="17"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="5">
+        <v>15</v>
+      </c>
+      <c r="B16" s="10"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="11"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="5">
+        <v>16</v>
+      </c>
+      <c r="B17" s="10"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="11"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="5">
+        <v>17</v>
+      </c>
+      <c r="B18" s="10"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="11"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="5">
+        <v>18</v>
+      </c>
+      <c r="B19" s="10"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="11"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="5">
+        <v>19</v>
+      </c>
+      <c r="B20" s="10"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="11"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="5">
+        <v>20</v>
+      </c>
+      <c r="B21" s="10"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="11"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="5">
+        <v>21</v>
+      </c>
+      <c r="B22" s="10"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="11"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="5">
+        <v>22</v>
+      </c>
+      <c r="B23" s="10"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="11"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="5">
+        <v>23</v>
+      </c>
+      <c r="B24" s="10"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="11"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="5">
+        <v>24</v>
+      </c>
+      <c r="B25" s="10"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="11"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="5">
+        <v>25</v>
+      </c>
+      <c r="B26" s="10"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="11"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="5">
+        <v>26</v>
+      </c>
+      <c r="B27" s="10"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="11"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="5">
+        <v>27</v>
+      </c>
+      <c r="B28" s="10"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="11"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="5">
+        <v>28</v>
+      </c>
+      <c r="B29" s="10"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="11"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="5">
+        <v>29</v>
+      </c>
+      <c r="B30" s="10"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="11"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="5">
+        <v>30</v>
+      </c>
+      <c r="B31" s="10"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="11"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="5">
+        <v>31</v>
+      </c>
+      <c r="B32" s="10"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="11"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="5">
+        <v>32</v>
+      </c>
+      <c r="B33" s="10"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="11"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="5">
+        <v>33</v>
+      </c>
+      <c r="B34" s="10"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="11"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="5">
+        <v>34</v>
+      </c>
+      <c r="B35" s="10"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="11"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="5">
+        <v>35</v>
+      </c>
+      <c r="B36" s="10"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="11"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="5">
+        <v>36</v>
+      </c>
+      <c r="B37" s="10"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="11"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="5">
+        <v>37</v>
+      </c>
+      <c r="B38" s="10"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="11"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="5">
+        <v>38</v>
+      </c>
+      <c r="B39" s="10"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="11"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="5">
+        <v>39</v>
+      </c>
+      <c r="B40" s="10"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="11"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="5">
+        <v>40</v>
+      </c>
+      <c r="B41" s="10"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="11"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="5">
+        <v>41</v>
+      </c>
+      <c r="B42" s="10"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="11"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="5">
+        <v>42</v>
+      </c>
+      <c r="B43" s="10"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="11"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="5">
+        <v>43</v>
+      </c>
+      <c r="B44" s="10"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="11"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="5">
+        <v>44</v>
+      </c>
+      <c r="B45" s="10"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="11"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="5">
+        <v>45</v>
+      </c>
+      <c r="B46" s="10"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="11"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="5">
+        <v>46</v>
+      </c>
+      <c r="B47" s="10"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="11"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="5">
+        <v>47</v>
+      </c>
+      <c r="B48" s="10"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="11"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="5">
+        <v>48</v>
+      </c>
+      <c r="B49" s="10"/>
+      <c r="C49" s="11"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="11"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="5">
+        <v>49</v>
+      </c>
+      <c r="B50" s="10"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="11"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="5">
+        <v>50</v>
+      </c>
+      <c r="B51" s="10"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="11"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="5">
+        <v>51</v>
+      </c>
+      <c r="B52" s="10"/>
+      <c r="C52" s="11"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="9"/>
+      <c r="F52" s="11"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="5">
+        <v>52</v>
+      </c>
+      <c r="B53" s="10"/>
+      <c r="C53" s="11"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="9"/>
+      <c r="F53" s="11"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="5">
+        <v>53</v>
+      </c>
+      <c r="B54" s="10"/>
+      <c r="C54" s="11"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="9"/>
+      <c r="F54" s="11"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" s="5">
+        <v>54</v>
+      </c>
+      <c r="B55" s="10"/>
+      <c r="C55" s="11"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="9"/>
+      <c r="F55" s="11"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="5">
+        <v>55</v>
+      </c>
+      <c r="B56" s="10"/>
+      <c r="C56" s="11"/>
+      <c r="D56" s="9"/>
+      <c r="E56" s="9"/>
+      <c r="F56" s="11"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" s="5">
+        <v>56</v>
+      </c>
+      <c r="B57" s="10"/>
+      <c r="C57" s="11"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="9"/>
+      <c r="F57" s="11"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" s="5">
+        <v>57</v>
+      </c>
+      <c r="B58" s="10"/>
+      <c r="C58" s="11"/>
+      <c r="D58" s="9"/>
+      <c r="E58" s="9"/>
+      <c r="F58" s="11"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" s="5">
+        <v>58</v>
+      </c>
+      <c r="B59" s="10"/>
+      <c r="C59" s="11"/>
+      <c r="D59" s="9"/>
+      <c r="E59" s="9"/>
+      <c r="F59" s="11"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" s="5">
+        <v>59</v>
+      </c>
+      <c r="B60" s="10"/>
+      <c r="C60" s="11"/>
+      <c r="D60" s="9"/>
+      <c r="E60" s="9"/>
+      <c r="F60" s="11"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" s="5">
+        <v>60</v>
+      </c>
+      <c r="B61" s="10"/>
+      <c r="C61" s="11"/>
+      <c r="D61" s="9"/>
+      <c r="E61" s="9"/>
+      <c r="F61" s="11"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" s="5">
+        <v>61</v>
+      </c>
+      <c r="B62" s="10"/>
+      <c r="C62" s="11"/>
+      <c r="D62" s="9"/>
+      <c r="E62" s="9"/>
+      <c r="F62" s="11"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" s="5">
+        <v>62</v>
+      </c>
+      <c r="B63" s="10"/>
+      <c r="C63" s="11"/>
+      <c r="D63" s="9"/>
+      <c r="E63" s="9"/>
+      <c r="F63" s="11"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" s="5">
+        <v>63</v>
+      </c>
+      <c r="B64" s="10"/>
+      <c r="C64" s="11"/>
+      <c r="D64" s="9"/>
+      <c r="E64" s="9"/>
+      <c r="F64" s="11"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" s="5">
+        <v>64</v>
+      </c>
+      <c r="B65" s="10"/>
+      <c r="C65" s="11"/>
+      <c r="D65" s="9"/>
+      <c r="E65" s="9"/>
+      <c r="F65" s="11"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" s="5">
+        <v>65</v>
+      </c>
+      <c r="B66" s="10"/>
+      <c r="C66" s="11"/>
+      <c r="D66" s="9"/>
+      <c r="E66" s="9"/>
+      <c r="F66" s="11"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" s="5">
+        <v>66</v>
+      </c>
+      <c r="B67" s="10"/>
+      <c r="C67" s="11"/>
+      <c r="D67" s="9"/>
+      <c r="E67" s="9"/>
+      <c r="F67" s="11"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" s="5">
+        <v>67</v>
+      </c>
+      <c r="B68" s="10"/>
+      <c r="C68" s="11"/>
+      <c r="D68" s="9"/>
+      <c r="E68" s="9"/>
+      <c r="F68" s="11"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" s="5">
+        <v>68</v>
+      </c>
+      <c r="B69" s="10"/>
+      <c r="C69" s="11"/>
+      <c r="D69" s="9"/>
+      <c r="E69" s="9"/>
+      <c r="F69" s="11"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" s="5">
+        <v>69</v>
+      </c>
+      <c r="B70" s="10"/>
+      <c r="C70" s="11"/>
+      <c r="D70" s="9"/>
+      <c r="E70" s="9"/>
+      <c r="F70" s="11"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71" s="5">
+        <v>70</v>
+      </c>
+      <c r="B71" s="10"/>
+      <c r="C71" s="11"/>
+      <c r="D71" s="9"/>
+      <c r="E71" s="9"/>
+      <c r="F71" s="11"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72" s="5">
+        <v>71</v>
+      </c>
+      <c r="B72" s="10"/>
+      <c r="C72" s="11"/>
+      <c r="D72" s="9"/>
+      <c r="E72" s="9"/>
+      <c r="F72" s="11"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73" s="5">
+        <v>72</v>
+      </c>
+      <c r="B73" s="10"/>
+      <c r="C73" s="11"/>
+      <c r="D73" s="9"/>
+      <c r="E73" s="9"/>
+      <c r="F73" s="11"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74" s="5">
+        <v>73</v>
+      </c>
+      <c r="B74" s="10"/>
+      <c r="C74" s="11"/>
+      <c r="D74" s="9"/>
+      <c r="E74" s="9"/>
+      <c r="F74" s="11"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A75" s="5">
+        <v>74</v>
+      </c>
+      <c r="B75" s="10"/>
+      <c r="C75" s="11"/>
+      <c r="D75" s="9"/>
+      <c r="E75" s="9"/>
+      <c r="F75" s="11"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A76" s="5">
+        <v>75</v>
+      </c>
+      <c r="B76" s="10"/>
+      <c r="C76" s="11"/>
+      <c r="D76" s="9"/>
+      <c r="E76" s="9"/>
+      <c r="F76" s="11"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77" s="5">
+        <v>76</v>
+      </c>
+      <c r="B77" s="10"/>
+      <c r="C77" s="11"/>
+      <c r="D77" s="9"/>
+      <c r="E77" s="9"/>
+      <c r="F77" s="11"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A78" s="5">
+        <v>77</v>
+      </c>
+      <c r="B78" s="10"/>
+      <c r="C78" s="11"/>
+      <c r="D78" s="9"/>
+      <c r="E78" s="9"/>
+      <c r="F78" s="11"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A79" s="5">
+        <v>78</v>
+      </c>
+      <c r="B79" s="10"/>
+      <c r="C79" s="11"/>
+      <c r="D79" s="9"/>
+      <c r="E79" s="9"/>
+      <c r="F79" s="11"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A80" s="5">
+        <v>79</v>
+      </c>
+      <c r="B80" s="10"/>
+      <c r="C80" s="11"/>
+      <c r="D80" s="9"/>
+      <c r="E80" s="9"/>
+      <c r="F80" s="11"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A81" s="5">
+        <v>80</v>
+      </c>
+      <c r="B81" s="10"/>
+      <c r="C81" s="11"/>
+      <c r="D81" s="9"/>
+      <c r="E81" s="9"/>
+      <c r="F81" s="11"/>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A82" s="5">
+        <v>81</v>
+      </c>
+      <c r="B82" s="10"/>
+      <c r="C82" s="11"/>
+      <c r="D82" s="9"/>
+      <c r="E82" s="9"/>
+      <c r="F82" s="11"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A83" s="5">
+        <v>82</v>
+      </c>
+      <c r="B83" s="10"/>
+      <c r="C83" s="11"/>
+      <c r="D83" s="9"/>
+      <c r="E83" s="9"/>
+      <c r="F83" s="11"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A84" s="5">
+        <v>83</v>
+      </c>
+      <c r="B84" s="10"/>
+      <c r="C84" s="11"/>
+      <c r="D84" s="9"/>
+      <c r="E84" s="9"/>
+      <c r="F84" s="11"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A85" s="5">
+        <v>84</v>
+      </c>
+      <c r="B85" s="10"/>
+      <c r="C85" s="11"/>
+      <c r="D85" s="9"/>
+      <c r="E85" s="9"/>
+      <c r="F85" s="11"/>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A86" s="5">
+        <v>85</v>
+      </c>
+      <c r="B86" s="10"/>
+      <c r="C86" s="11"/>
+      <c r="D86" s="9"/>
+      <c r="E86" s="9"/>
+      <c r="F86" s="11"/>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A87" s="5">
+        <v>86</v>
+      </c>
+      <c r="B87" s="10"/>
+      <c r="C87" s="11"/>
+      <c r="D87" s="9"/>
+      <c r="E87" s="9"/>
+      <c r="F87" s="11"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A88" s="5">
+        <v>87</v>
+      </c>
+      <c r="B88" s="10"/>
+      <c r="C88" s="11"/>
+      <c r="D88" s="9"/>
+      <c r="E88" s="9"/>
+      <c r="F88" s="11"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A89" s="5">
+        <v>88</v>
+      </c>
+      <c r="B89" s="10"/>
+      <c r="C89" s="11"/>
+      <c r="D89" s="9"/>
+      <c r="E89" s="9"/>
+      <c r="F89" s="11"/>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A90" s="5">
+        <v>89</v>
+      </c>
+      <c r="B90" s="10"/>
+      <c r="C90" s="11"/>
+      <c r="D90" s="9"/>
+      <c r="E90" s="9"/>
+      <c r="F90" s="11"/>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A91" s="5">
+        <v>90</v>
+      </c>
+      <c r="B91" s="10"/>
+      <c r="C91" s="11"/>
+      <c r="D91" s="9"/>
+      <c r="E91" s="9"/>
+      <c r="F91" s="11"/>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A92" s="5">
+        <v>91</v>
+      </c>
+      <c r="B92" s="10"/>
+      <c r="C92" s="11"/>
+      <c r="D92" s="9"/>
+      <c r="E92" s="9"/>
+      <c r="F92" s="11"/>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A93" s="5">
+        <v>92</v>
+      </c>
+      <c r="B93" s="10"/>
+      <c r="C93" s="11"/>
+      <c r="D93" s="9"/>
+      <c r="E93" s="9"/>
+      <c r="F93" s="11"/>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A94" s="5">
+        <v>93</v>
+      </c>
+      <c r="B94" s="10"/>
+      <c r="C94" s="11"/>
+      <c r="D94" s="9"/>
+      <c r="E94" s="9"/>
+      <c r="F94" s="11"/>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A95" s="5">
+        <v>94</v>
+      </c>
+      <c r="B95" s="10"/>
+      <c r="C95" s="11"/>
+      <c r="D95" s="9"/>
+      <c r="E95" s="9"/>
+      <c r="F95" s="11"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <mergeCells count="39">
-    <mergeCell ref="A2"/>
-    <mergeCell ref="B2"/>
-    <mergeCell ref="C2"/>
-    <mergeCell ref="A4"/>
-    <mergeCell ref="B4"/>
-    <mergeCell ref="C4"/>
-    <mergeCell ref="A3"/>
-    <mergeCell ref="B3"/>
-    <mergeCell ref="C3"/>
-    <mergeCell ref="A6"/>
-    <mergeCell ref="B6"/>
-    <mergeCell ref="C6"/>
-    <mergeCell ref="A5"/>
-    <mergeCell ref="B5"/>
-    <mergeCell ref="C5"/>
-    <mergeCell ref="A8"/>
-    <mergeCell ref="B8"/>
-    <mergeCell ref="C8"/>
-    <mergeCell ref="A7"/>
-    <mergeCell ref="B7"/>
-    <mergeCell ref="C7"/>
-    <mergeCell ref="A10"/>
-    <mergeCell ref="B10"/>
-    <mergeCell ref="C10"/>
-    <mergeCell ref="A9"/>
-    <mergeCell ref="B9"/>
-    <mergeCell ref="C9"/>
-    <mergeCell ref="A12"/>
-    <mergeCell ref="B12"/>
-    <mergeCell ref="C12"/>
-    <mergeCell ref="A11"/>
-    <mergeCell ref="B11"/>
-    <mergeCell ref="C11"/>
-    <mergeCell ref="A14"/>
-    <mergeCell ref="B14"/>
-    <mergeCell ref="C14"/>
-    <mergeCell ref="A13"/>
-    <mergeCell ref="B13"/>
-    <mergeCell ref="C13"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>